<commit_message>
Your branch is up to date with 'origin/master'.
</commit_message>
<xml_diff>
--- a/Recordsfiles/Covod-19 data.xlsx
+++ b/Recordsfiles/Covod-19 data.xlsx
@@ -148,13 +148,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -360,10 +362,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>5206</c:v>
+                  <c:v>5384</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3253</c:v>
+                  <c:v>3431</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1823</c:v>
@@ -428,11 +430,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="189860656"/>
-        <c:axId val="189863008"/>
+        <c:axId val="192807920"/>
+        <c:axId val="192805176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="189860656"/>
+        <c:axId val="192807920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -475,7 +477,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189863008"/>
+        <c:crossAx val="192805176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -483,7 +485,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="189863008"/>
+        <c:axId val="192805176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -534,7 +536,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="189860656"/>
+        <c:crossAx val="192807920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1459,10 +1461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:O300"/>
+  <dimension ref="A2:O300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H113" sqref="H113"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="I104" sqref="I104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,20 +1480,20 @@
     <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" ht="27" x14ac:dyDescent="0.35">
-      <c r="G2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-    </row>
-    <row r="5" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="27" x14ac:dyDescent="0.35">
+      <c r="G2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+    </row>
+    <row r="5" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
@@ -1519,7 +1521,10 @@
       </c>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
       <c r="B6" s="3">
         <v>43905</v>
       </c>
@@ -1532,24 +1537,27 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="G6" s="7">
+      <c r="G6" s="9">
         <f>SUM(C6:C3000)</f>
-        <v>5206</v>
-      </c>
-      <c r="H6" s="8">
+        <v>5384</v>
+      </c>
+      <c r="H6" s="10">
         <f>G6-(I6+J6)</f>
-        <v>3253</v>
-      </c>
-      <c r="I6" s="9">
+        <v>3431</v>
+      </c>
+      <c r="I6" s="11">
         <f>SUM(D6:D3000)</f>
         <v>1823</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="12">
         <f>SUM(E6:E3000)</f>
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
       <c r="B7" s="3">
         <v>43906</v>
       </c>
@@ -1562,12 +1570,15 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="9"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
       <c r="B8" s="3">
         <v>43907</v>
       </c>
@@ -1581,7 +1592,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
       <c r="B9" s="3">
         <v>43908</v>
       </c>
@@ -1595,7 +1609,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
       <c r="B10" s="3">
         <v>43909</v>
       </c>
@@ -1609,7 +1626,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
       <c r="B11" s="3">
         <v>43910</v>
       </c>
@@ -1623,7 +1643,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
       <c r="B12" s="3">
         <v>43911</v>
       </c>
@@ -1637,7 +1660,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
       <c r="B13" s="3">
         <v>43912</v>
       </c>
@@ -1651,7 +1677,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>9</v>
+      </c>
       <c r="B14" s="3">
         <v>43913</v>
       </c>
@@ -1665,7 +1694,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>10</v>
+      </c>
       <c r="B15" s="3">
         <v>43914</v>
       </c>
@@ -1679,7 +1711,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>11</v>
+      </c>
       <c r="B16" s="3">
         <v>43915</v>
       </c>
@@ -1693,7 +1728,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>12</v>
+      </c>
       <c r="B17" s="3">
         <v>43916</v>
       </c>
@@ -1707,7 +1745,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>13</v>
+      </c>
       <c r="B18" s="3">
         <v>43917</v>
       </c>
@@ -1721,7 +1762,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>14</v>
+      </c>
       <c r="B19" s="3">
         <v>43918</v>
       </c>
@@ -1735,7 +1779,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>15</v>
+      </c>
       <c r="B20" s="3">
         <v>43919</v>
       </c>
@@ -1749,21 +1796,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>16</v>
+      </c>
+      <c r="B21" s="7">
         <v>43920</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="6">
         <v>8</v>
       </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>17</v>
+      </c>
       <c r="B22" s="3">
         <v>43921</v>
       </c>
@@ -1777,7 +1830,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
       <c r="B23" s="3">
         <v>43922</v>
       </c>
@@ -1791,7 +1847,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>19</v>
+      </c>
       <c r="B24" s="3">
         <v>43923</v>
       </c>
@@ -1805,7 +1864,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>20</v>
+      </c>
       <c r="B25" s="3">
         <v>43924</v>
       </c>
@@ -1819,7 +1881,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>21</v>
+      </c>
       <c r="B26" s="3">
         <v>43925</v>
       </c>
@@ -1833,7 +1898,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>22</v>
+      </c>
       <c r="B27" s="3">
         <v>43926</v>
       </c>
@@ -1847,7 +1915,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>23</v>
+      </c>
       <c r="B28" s="3">
         <v>43927</v>
       </c>
@@ -1861,7 +1932,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>24</v>
+      </c>
       <c r="B29" s="3">
         <v>43928</v>
       </c>
@@ -1875,7 +1949,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>25</v>
+      </c>
       <c r="B30" s="3">
         <v>43929</v>
       </c>
@@ -1889,7 +1966,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>26</v>
+      </c>
       <c r="B31" s="3">
         <v>43930</v>
       </c>
@@ -1903,7 +1983,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>27</v>
+      </c>
       <c r="B32" s="3">
         <v>43931</v>
       </c>
@@ -1917,7 +2000,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>28</v>
+      </c>
       <c r="B33" s="3">
         <v>43932</v>
       </c>
@@ -1931,7 +2017,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>29</v>
+      </c>
       <c r="B34" s="3">
         <v>43933</v>
       </c>
@@ -1945,7 +2034,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>30</v>
+      </c>
       <c r="B35" s="3">
         <v>43934</v>
       </c>
@@ -1959,7 +2051,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>31</v>
+      </c>
       <c r="B36" s="3">
         <v>43935</v>
       </c>
@@ -1973,7 +2068,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>32</v>
+      </c>
       <c r="B37" s="3">
         <v>43936</v>
       </c>
@@ -1987,7 +2085,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>33</v>
+      </c>
       <c r="B38" s="3">
         <v>43937</v>
       </c>
@@ -2001,7 +2102,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>34</v>
+      </c>
       <c r="B39" s="3">
         <v>43938</v>
       </c>
@@ -2015,7 +2119,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>35</v>
+      </c>
       <c r="B40" s="3">
         <v>43939</v>
       </c>
@@ -2029,7 +2136,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>36</v>
+      </c>
       <c r="B41" s="3">
         <v>43940</v>
       </c>
@@ -2043,7 +2153,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>37</v>
+      </c>
       <c r="B42" s="3">
         <v>43941</v>
       </c>
@@ -2057,7 +2170,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>37</v>
+      </c>
       <c r="B43" s="3">
         <v>43942</v>
       </c>
@@ -2071,7 +2187,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>38</v>
+      </c>
       <c r="B44" s="3">
         <v>43943</v>
       </c>
@@ -2085,7 +2204,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>40</v>
+      </c>
       <c r="B45" s="3">
         <v>43944</v>
       </c>
@@ -2099,7 +2221,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>41</v>
+      </c>
       <c r="B46" s="3">
         <v>43945</v>
       </c>
@@ -2113,7 +2238,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>42</v>
+      </c>
       <c r="B47" s="3">
         <v>43946</v>
       </c>
@@ -2127,7 +2255,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>43</v>
+      </c>
       <c r="B48" s="3">
         <v>43947</v>
       </c>
@@ -2141,7 +2272,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>44</v>
+      </c>
       <c r="B49" s="3">
         <v>43948</v>
       </c>
@@ -2155,7 +2289,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>45</v>
+      </c>
       <c r="B50" s="3">
         <v>43949</v>
       </c>
@@ -2169,7 +2306,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>46</v>
+      </c>
       <c r="B51" s="3">
         <v>43950</v>
       </c>
@@ -2183,7 +2323,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>47</v>
+      </c>
       <c r="B52" s="3">
         <v>43951</v>
       </c>
@@ -2197,7 +2340,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>48</v>
+      </c>
       <c r="B53" s="3">
         <v>43952</v>
       </c>
@@ -2211,7 +2357,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>49</v>
+      </c>
       <c r="B54" s="3">
         <v>43953</v>
       </c>
@@ -2225,7 +2374,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>50</v>
+      </c>
       <c r="B55" s="3">
         <v>43954</v>
       </c>
@@ -2239,7 +2391,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>51</v>
+      </c>
       <c r="B56" s="3">
         <v>43955</v>
       </c>
@@ -2253,7 +2408,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>52</v>
+      </c>
       <c r="B57" s="3">
         <v>43956</v>
       </c>
@@ -2267,7 +2425,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>53</v>
+      </c>
       <c r="B58" s="3">
         <v>43957</v>
       </c>
@@ -2281,7 +2442,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>54</v>
+      </c>
       <c r="B59" s="3">
         <v>43958</v>
       </c>
@@ -2295,7 +2459,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>55</v>
+      </c>
       <c r="B60" s="3">
         <v>43959</v>
       </c>
@@ -2309,7 +2476,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>56</v>
+      </c>
       <c r="B61" s="3">
         <v>43960</v>
       </c>
@@ -2323,7 +2493,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>57</v>
+      </c>
       <c r="B62" s="3">
         <v>43961</v>
       </c>
@@ -2337,7 +2510,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>58</v>
+      </c>
       <c r="B63" s="3">
         <v>43962</v>
       </c>
@@ -2351,7 +2527,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>59</v>
+      </c>
       <c r="B64" s="3">
         <v>43963</v>
       </c>
@@ -2365,7 +2544,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>60</v>
+      </c>
       <c r="B65" s="3">
         <v>43964</v>
       </c>
@@ -2379,7 +2561,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>61</v>
+      </c>
       <c r="B66" s="3">
         <v>43965</v>
       </c>
@@ -2393,7 +2578,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>62</v>
+      </c>
       <c r="B67" s="3">
         <v>43966</v>
       </c>
@@ -2407,7 +2595,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>63</v>
+      </c>
       <c r="B68" s="3">
         <v>43967</v>
       </c>
@@ -2421,7 +2612,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>64</v>
+      </c>
       <c r="B69" s="3">
         <v>43968</v>
       </c>
@@ -2435,7 +2629,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>65</v>
+      </c>
       <c r="B70" s="3">
         <v>43969</v>
       </c>
@@ -2449,7 +2646,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>66</v>
+      </c>
       <c r="B71" s="3">
         <v>43970</v>
       </c>
@@ -2463,7 +2663,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>67</v>
+      </c>
       <c r="B72" s="3">
         <v>43971</v>
       </c>
@@ -2477,7 +2680,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>68</v>
+      </c>
       <c r="B73" s="3">
         <v>43972</v>
       </c>
@@ -2491,7 +2697,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>69</v>
+      </c>
       <c r="B74" s="3">
         <v>43973</v>
       </c>
@@ -2505,7 +2714,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>70</v>
+      </c>
       <c r="B75" s="3">
         <v>43974</v>
       </c>
@@ -2519,7 +2731,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>71</v>
+      </c>
       <c r="B76" s="3">
         <v>43975</v>
       </c>
@@ -2533,7 +2748,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>72</v>
+      </c>
       <c r="B77" s="3">
         <v>43976</v>
       </c>
@@ -2547,7 +2765,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>73</v>
+      </c>
       <c r="B78" s="3">
         <v>43977</v>
       </c>
@@ -2561,7 +2782,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>74</v>
+      </c>
       <c r="B79" s="3">
         <v>43978</v>
       </c>
@@ -2575,7 +2799,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>75</v>
+      </c>
       <c r="B80" s="3">
         <v>43979</v>
       </c>
@@ -2589,7 +2816,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>76</v>
+      </c>
       <c r="B81" s="3">
         <v>43980</v>
       </c>
@@ -2603,7 +2833,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>77</v>
+      </c>
       <c r="B82" s="3">
         <v>43981</v>
       </c>
@@ -2617,7 +2850,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>78</v>
+      </c>
       <c r="B83" s="3">
         <v>43982</v>
       </c>
@@ -2631,7 +2867,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>79</v>
+      </c>
       <c r="B84" s="3">
         <v>43983</v>
       </c>
@@ -2645,7 +2884,10 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>80</v>
+      </c>
       <c r="B85" s="3">
         <v>43984</v>
       </c>
@@ -2659,7 +2901,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>81</v>
+      </c>
       <c r="B86" s="3">
         <v>43985</v>
       </c>
@@ -2673,7 +2918,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>82</v>
+      </c>
       <c r="B87" s="3">
         <v>43986</v>
       </c>
@@ -2687,7 +2935,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>83</v>
+      </c>
       <c r="B88" s="3">
         <v>43987</v>
       </c>
@@ -2701,7 +2952,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>84</v>
+      </c>
       <c r="B89" s="3">
         <v>43988</v>
       </c>
@@ -2715,7 +2969,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>85</v>
+      </c>
       <c r="B90" s="3">
         <v>43989</v>
       </c>
@@ -2729,7 +2986,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>86</v>
+      </c>
       <c r="B91" s="3">
         <v>43990</v>
       </c>
@@ -2743,7 +3003,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>87</v>
+      </c>
       <c r="B92" s="3">
         <v>43991</v>
       </c>
@@ -2757,7 +3020,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>88</v>
+      </c>
       <c r="B93" s="3">
         <v>43992</v>
       </c>
@@ -2771,7 +3037,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>89</v>
+      </c>
       <c r="B94" s="3">
         <v>43993</v>
       </c>
@@ -2785,7 +3054,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>90</v>
+      </c>
       <c r="B95" s="3">
         <v>43994</v>
       </c>
@@ -2799,7 +3071,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>91</v>
+      </c>
       <c r="B96" s="3">
         <v>43995</v>
       </c>
@@ -2813,7 +3088,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>92</v>
+      </c>
       <c r="B97" s="3">
         <v>43996</v>
       </c>
@@ -2827,7 +3105,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>93</v>
+      </c>
       <c r="B98" s="3">
         <v>43997</v>
       </c>
@@ -2841,7 +3122,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>94</v>
+      </c>
       <c r="B99" s="3">
         <v>43998</v>
       </c>
@@ -2855,7 +3139,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>95</v>
+      </c>
       <c r="B100" s="3">
         <v>43999</v>
       </c>
@@ -2869,7 +3156,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>96</v>
+      </c>
       <c r="B101" s="3">
         <v>44000</v>
       </c>
@@ -2883,7 +3173,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>97</v>
+      </c>
       <c r="B102" s="3">
         <v>43849</v>
       </c>
@@ -2897,7 +3190,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>98</v>
+      </c>
       <c r="B103" s="3">
         <v>44002</v>
       </c>
@@ -2911,7 +3207,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>99</v>
+      </c>
       <c r="B104" s="3">
         <v>44003</v>
       </c>
@@ -2925,7 +3224,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>100</v>
+      </c>
       <c r="B105" s="3">
         <v>44004</v>
       </c>
@@ -2939,7 +3241,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>101</v>
+      </c>
       <c r="B106" s="3">
         <v>44005</v>
       </c>
@@ -2953,7 +3258,10 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107">
+        <v>102</v>
+      </c>
       <c r="B107" s="3">
         <v>44006</v>
       </c>
@@ -2967,19 +3275,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B108" s="3"/>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108">
+        <v>103</v>
+      </c>
+      <c r="B108" s="3">
+        <v>44007</v>
+      </c>
+      <c r="C108">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B109" s="3"/>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B110" s="3"/>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B111" s="3"/>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B112" s="3"/>
     </row>
     <row r="113" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
New file:   README.md.txt 	modified:   Recordsfiles/Covod-19 data.xlsx
</commit_message>
<xml_diff>
--- a/Recordsfiles/Covod-19 data.xlsx
+++ b/Recordsfiles/Covod-19 data.xlsx
@@ -661,16 +661,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>14168</c:v>
+                  <c:v>15601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7660</c:v>
+                  <c:v>8203</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6258</c:v>
+                  <c:v>7135</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>250</c:v>
+                  <c:v>263</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -729,11 +729,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="373448976"/>
-        <c:axId val="373449368"/>
+        <c:axId val="150327560"/>
+        <c:axId val="150331088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="373448976"/>
+        <c:axId val="150327560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -776,7 +776,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373449368"/>
+        <c:crossAx val="150331088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -784,7 +784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="373449368"/>
+        <c:axId val="150331088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -835,7 +835,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="373448976"/>
+        <c:crossAx val="150327560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1762,8 +1762,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L121" workbookViewId="0">
-      <selection activeCell="Q133" sqref="Q133"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O135" sqref="O135:O136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1874,19 +1874,19 @@
       </c>
       <c r="I6" s="23">
         <f>SUM(C6:C3000)</f>
-        <v>14168</v>
+        <v>15601</v>
       </c>
       <c r="J6" s="24">
         <f>I6-(K6+L6)</f>
-        <v>7660</v>
+        <v>8203</v>
       </c>
       <c r="K6" s="25">
         <f>SUM(D6:D3000)</f>
-        <v>6258</v>
+        <v>7135</v>
       </c>
       <c r="L6" s="26">
         <f>SUM(E6:E3000)</f>
-        <v>250</v>
+        <v>263</v>
       </c>
       <c r="N6" t="str">
         <f>CONCATENATE($Q$6,$R$5,"'",A6,"'",$R$5,$Q$5,F6,$Q$5,H6,$R$6)</f>
@@ -1974,11 +1974,11 @@
       </c>
       <c r="K8" s="17">
         <f>(K6/I6)</f>
-        <v>0.44169960474308301</v>
+        <v>0.45734247804627909</v>
       </c>
       <c r="L8" s="17">
         <f>(L6/I6)</f>
-        <v>1.7645398080180688E-2</v>
+        <v>1.6857893724761232E-2</v>
       </c>
       <c r="N8" t="str">
         <f t="shared" si="0"/>
@@ -4666,7 +4666,7 @@
         <v>64</v>
       </c>
       <c r="N71" t="str">
-        <f t="shared" ref="N71:N134" si="7">CONCATENATE($Q$6,$R$5,"'",A71,"'",$R$5,$Q$5,F71,$Q$5,H71,$R$6)</f>
+        <f t="shared" ref="N71:N135" si="7">CONCATENATE($Q$6,$R$5,"'",A71,"'",$R$5,$Q$5,F71,$Q$5,H71,$R$6)</f>
         <v>['66',963,50]</v>
       </c>
       <c r="O71" t="str">
@@ -4700,7 +4700,7 @@
         <v>349</v>
       </c>
       <c r="H72" s="11">
-        <f t="shared" ref="H72:H134" si="11">H71+E72</f>
+        <f t="shared" ref="H72:H135" si="11">H71+E72</f>
         <v>50</v>
       </c>
       <c r="J72" s="19">
@@ -6266,11 +6266,11 @@
         <v>4</v>
       </c>
       <c r="F113" s="13">
-        <f t="shared" ref="F113:F134" si="13">F112+C113</f>
+        <f t="shared" ref="F113:F136" si="13">F112+C113</f>
         <v>6366</v>
       </c>
       <c r="G113" s="12">
-        <f t="shared" ref="G113:G134" si="14">G112+D113</f>
+        <f t="shared" ref="G113:H136" si="14">G112+D113</f>
         <v>2039</v>
       </c>
       <c r="H113" s="11">
@@ -6282,7 +6282,7 @@
         <v>['108',6366,148]</v>
       </c>
       <c r="O113" t="str">
-        <f t="shared" ref="O113:O134" si="15">CONCATENATE($Q$6,$R$5,"'",A113,"'",$R$5,$Q$5,F113,$Q$5,G113,$R$6)</f>
+        <f t="shared" ref="O113:O136" si="15">CONCATENATE($Q$6,$R$5,"'",A113,"'",$R$5,$Q$5,F113,$Q$5,G113,$R$6)</f>
         <v>['108',6366,2039]</v>
       </c>
     </row>
@@ -7064,10 +7064,78 @@
       </c>
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B135" s="3"/>
+      <c r="A135">
+        <v>130</v>
+      </c>
+      <c r="B135" s="3">
+        <v>44034</v>
+      </c>
+      <c r="C135">
+        <v>637</v>
+      </c>
+      <c r="D135">
+        <v>499</v>
+      </c>
+      <c r="E135">
+        <v>10</v>
+      </c>
+      <c r="F135" s="13">
+        <f t="shared" si="13"/>
+        <v>14805</v>
+      </c>
+      <c r="G135" s="12">
+        <f t="shared" si="14"/>
+        <v>6757</v>
+      </c>
+      <c r="H135" s="11">
+        <f t="shared" si="11"/>
+        <v>260</v>
+      </c>
+      <c r="N135" t="str">
+        <f t="shared" si="7"/>
+        <v>['130',14805,260]</v>
+      </c>
+      <c r="O135" t="str">
+        <f t="shared" si="15"/>
+        <v>['130',14805,6757]</v>
+      </c>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B136" s="3"/>
+      <c r="A136">
+        <v>131</v>
+      </c>
+      <c r="B136" s="3">
+        <v>44035</v>
+      </c>
+      <c r="C136">
+        <v>796</v>
+      </c>
+      <c r="D136">
+        <v>378</v>
+      </c>
+      <c r="E136">
+        <v>3</v>
+      </c>
+      <c r="F136" s="13">
+        <f t="shared" si="13"/>
+        <v>15601</v>
+      </c>
+      <c r="G136" s="12">
+        <f t="shared" si="14"/>
+        <v>7135</v>
+      </c>
+      <c r="H136" s="11">
+        <f t="shared" si="14"/>
+        <v>263</v>
+      </c>
+      <c r="N136" t="str">
+        <f t="shared" ref="N136" si="16">CONCATENATE($Q$6,$R$5,"'",A136,"'",$R$5,$Q$5,F136,$Q$5,H136,$R$6)</f>
+        <v>['131',15601,263]</v>
+      </c>
+      <c r="O136" t="str">
+        <f t="shared" si="15"/>
+        <v>['131',15601,7135]</v>
+      </c>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B137" s="3"/>

</xml_diff>